<commit_message>
Shop - Purchase UI
</commit_message>
<xml_diff>
--- a/Assets/Resources/Data/Dialog.xlsx
+++ b/Assets/Resources/Data/Dialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Unity\capstone-2023-03\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A9A7D3-A1C8-4919-9E9C-402379099167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E861814-C0D0-41A2-A860-212BD26D8C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{E3E339C2-427C-46D8-B0F4-47F04CF9523A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Dialog!$A$1:$D$55</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Dialog!$A$1:$D$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,13 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="77">
-  <si>
-    <t>상점 주인</t>
-  </si>
-  <si>
-    <t>저는 상점 주인입니다</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -366,6 +360,18 @@
   </si>
   <si>
     <t>방에 들어와 보니, 갑자기 내 시청자들이 카드 구매에 필요한 돈을 바치겠다고 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상점주인 릴리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴리의 카드 상점에 오신 걸 환영합니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한번 보고 가시겠어요? 돈만 있으면 레어한 카드들도 얼마든지 살 수 있답니다! \n그리고 필요없는 카드를 처리 비용을 받고 버려주는 일도 하고 있어요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,10 +461,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}" name="Dialog" displayName="Dialog" ref="A1:D55" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D55" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D55">
-    <sortCondition ref="A1:A55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}" name="Dialog" displayName="Dialog" ref="A1:D56" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D56" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D56">
+    <sortCondition ref="A1:A56"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1B7DBA41-96C3-4CE3-B474-58352C79090C}" uniqueName="1" name="index" queryTableFieldId="1"/>
@@ -767,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FB65A4-AFB1-47B1-836C-30EB70945D8C}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -784,16 +790,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -801,13 +807,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -815,13 +821,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -829,13 +835,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -843,13 +849,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -857,13 +863,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -871,13 +877,13 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -885,13 +891,13 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -899,13 +905,13 @@
         <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -913,13 +919,13 @@
         <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -927,13 +933,13 @@
         <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -941,65 +947,65 @@
         <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>300</v>
+        <v>200</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>300</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>301</v>
+        <v>300</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>303</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
+        <v>302</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
@@ -1007,13 +1013,13 @@
         <v>303</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
@@ -1021,367 +1027,367 @@
         <v>303</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
         <v>57</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>304</v>
       </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>305</v>
+        <v>304</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>305</v>
       </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
-      </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24">
-        <v>306</v>
+        <v>305</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>306</v>
       </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
         <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29">
-        <v>400</v>
+        <v>309</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>400</v>
       </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31">
-        <v>1000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" t="s">
-        <v>25</v>
+        <v>400</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36">
-        <v>2000</v>
+        <v>1004</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41">
-        <v>3000</v>
+        <v>2004</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46">
-        <v>4100</v>
+        <v>3004</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
@@ -1389,125 +1395,139 @@
         <v>4100</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
         <v>13</v>
-      </c>
-      <c r="D47" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48">
-        <v>4101</v>
+        <v>4100</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49">
-        <v>4102</v>
+        <v>4101</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50">
-        <v>4103</v>
+        <v>4102</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51">
-        <v>4104</v>
+        <v>4103</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52">
-        <v>5100</v>
+        <v>4104</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53">
-        <v>5101</v>
+        <v>5100</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54">
-        <v>5102</v>
+        <v>5101</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55">
+        <v>5102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A56">
         <v>5103</v>
       </c>
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" t="s">
-        <v>54</v>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dialog & Standing CG
</commit_message>
<xml_diff>
--- a/Assets/Resources/Data/Dialog.xlsx
+++ b/Assets/Resources/Data/Dialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Unity\capstone-2023-03\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E861814-C0D0-41A2-A860-212BD26D8C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B41968-A558-41C3-B00A-25E0F6AC1EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{E3E339C2-427C-46D8-B0F4-47F04CF9523A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Dialog!$A$1:$D$56</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Dialog!$A$1:$D$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
   </si>
   <si>
     <t>Enemy1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -91,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>쉬고 가시는 것도 중요하죠. 잠시 편히 쉬어가세요, 여기서 여러분의 상처를 치료해 드릴게요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>세리나</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,18 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>트수들아 미안해~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크윽 개강해</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영입이라고? 뭐 나야 나쁠 거 없지!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>해적선장 마린</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -135,154 +115,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>최종 보스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드루이드 보스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성녀 보스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대충 해적 보스다 전투 돌입합니다!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메카닉 보스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무명 시참자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해적단 부하</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드루이드 부하</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성기사단 부하</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>메카닉 기계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>드루이드 부하 잡몹 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메카닉 부하 잡몹 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성녀 부하 잡몹 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해적선장 부하 잡몹 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>메카닉 체키</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아이돌 아이리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반형 부하 잡몹 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 협상 시도 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 전투 돌입 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 협상 실패 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해적단 협상 시도 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드루이드 협상 시도 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성기사단 협상 시도 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메카닉 협상 시도 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해적단 전투 돌입 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드루이드 전투 돌입 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성기사단 전투 돌입 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메카닉 전투 돌입 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해적단 협상 실패 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드루이드 협상 실패 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성기사단 협상 실패 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메카닉 협상 실패 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드루이드 패배 대사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성녀 패배 대사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메카닉 패배 대사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이돌 패배 대사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이돌 아이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -347,18 +187,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>혹시 이곳에서 같이 싸우게 해 주실 수 있나요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>폭렬!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>뭐임?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>방에 들어와 보니, 갑자기 내 시청자들이 카드 구매에 필요한 돈을 바치겠다고 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -372,6 +204,282 @@
   </si>
   <si>
     <t>한번 보고 가시겠어요? 돈만 있으면 레어한 카드들도 얼마든지 살 수 있답니다! \n그리고 필요없는 카드를 처리 비용을 받고 버려주는 일도 하고 있어요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수인 시청자</t>
+  </si>
+  <si>
+    <t>수인 시청자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이돌 루비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시청자로서 아이리님의 이번 대회 재밌게 지켜보고 있었습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 대회 기간 동안 같이 싸우게 해 주실 수 있나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partner1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물론이지! 새로운 동료는 언제나 환영이야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partner2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partner3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무명 스트리머</t>
+  </si>
+  <si>
+    <t>무명 스트리머</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마린 해적단 부하</t>
+  </si>
+  <si>
+    <t>마린 해적단 부하</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성녀의 신도</t>
+  </si>
+  <si>
+    <t>성녀의 신도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크윽... 개강해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미안 시청자들. 나는 여기까지인 것 같아.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>같이 싸우자고? 뭐 나야 나쁠 거 없지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(너무나도 동료로 참가하고 싶다는 표정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nurse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 부하들을 뚫고 여기까지 온 걸 보니 상당한 강자인 것 같네.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 내가 상대인 이상, 지금까지의 요행은 기대할 수 없을거야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리샤님의 우승을 위해 너는 여기서 죽어줘야겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거기까지다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대지여... 용서해 주십시오. 내가 충분히 힘을 발휘하지 못해 우리의 가호를 잃었습니다…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리의 언어가 결합되어 하나가 되었습니다. 이것이 바로 자연의 조화입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자연의 균형을 유지하기 위해, 나는 싸울 것입니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 세계의 조화를 어지럽히려는 어리석은 자가 있군요…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신의 가호가 우리와 함께하길.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐, 그것도 나쁘지 않겠지… 내 로봇들의 힘을 계속 보여줄 수 있으니.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아직 기술이 부족한 것 같네. 다음 대회까지 개선할 부분이 많겠어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아직 빛이 가득차지 않았나 보군요...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 또한 신의 뜻이겠지요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콘솔 준비 완료, 내 로봇들이 당신을 기다리고 있어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그 컨셉 어려울 것 같은데, 되게 잘 지키는구나.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요행인지 아닌지는 대봐야 아는 거겠죠!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으음, 그러니까… 제 마법이 신의 가호같은 것보다 강해요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과학은 마법을 이길 수 없다는 걸 보여드리죠!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 라이브는… 이것으로 종료야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음으로 내 제물이 될 사람이 너구나? 무대를 시작할 준비는 됐어?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대회에 참가하느라 많이 지쳐 보이네요. 이곳은 중립지역이니 잠시 편히 쉬어가세요. \n상처도 치료해 드릴게요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>...나는 나보다 강한 자의 편이다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어쩔 수 없군.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물론이죠! 수많은 시청자들의 응원을 받으며 여기까지 왔으니… \n반드시 이기겠습니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반가워~ 내가 이 'ROAD TO V' 대회의 주최자이자, '최종 보스' 역할을 맡고 있는 아이돌 루비야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[거부 프로토콜 활성화] 협상 불가능, 명령어 무시.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[승인 프로토콜 활성화] 협상 승인, 조건 수용.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">플랜에 방해가 될 참가자 발견. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[전투 프로토콜 활성화] 처리 모드로 이행합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전투를 시작하지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 대회에서 우승해서 꼭 유명한 버추얼 스트리머가 되고 말겠어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그러기 위해서… 승부다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역시 안정적으로 시청자를 더 벌기 위해서는 동료가 되는 수밖에...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근데 너 약하잖아. 내가 왜 협상을 해야 하지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그 정도로 마린 선장님에 대한 내 마음을 돌릴 순 없다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거부하지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 마린 선장님의 충실한 부하!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이곳은 성녀 리샤님의 영토다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">너희 같은 이단자와 협상할 이유는 없다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너는 여기서 끝이다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>...죄송합니다 성녀님</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -461,10 +569,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}" name="Dialog" displayName="Dialog" ref="A1:D56" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D56" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D56">
-    <sortCondition ref="A1:A56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}" name="Dialog" displayName="Dialog" ref="A1:D66" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D66" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
+    <sortCondition ref="A1:A66"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1B7DBA41-96C3-4CE3-B474-58352C79090C}" uniqueName="1" name="index" queryTableFieldId="1"/>
@@ -773,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FB65A4-AFB1-47B1-836C-30EB70945D8C}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -799,7 +907,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -810,10 +918,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -824,10 +932,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -835,13 +943,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -849,13 +957,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -863,13 +971,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -877,592 +985,592 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>200</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>300</v>
+        <v>102</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>300</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>301</v>
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>302</v>
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18">
-        <v>303</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
-        <v>303</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
-        <v>303</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>304</v>
+        <v>200</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>304</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
+        <v>300</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>305</v>
+        <v>300</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24">
-        <v>305</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
+        <v>301</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29">
-        <v>309</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>70</v>
+        <v>304</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30">
-        <v>400</v>
+        <v>304</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31">
-        <v>400</v>
+        <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32">
-        <v>1000</v>
+        <v>305</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>1001</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>24</v>
+        <v>306</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34">
-        <v>1002</v>
+        <v>306</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35">
-        <v>1003</v>
+        <v>307</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36">
-        <v>1004</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37">
-        <v>2000</v>
+        <v>307</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>2001</v>
+        <v>308</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39">
-        <v>2002</v>
+        <v>309</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40">
-        <v>2003</v>
+        <v>400</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41">
-        <v>2004</v>
-      </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>27</v>
+        <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43">
-        <v>3001</v>
+        <v>1001</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44">
-        <v>3002</v>
+        <v>1002</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45">
-        <v>3003</v>
+        <v>1003</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46">
-        <v>3004</v>
+        <v>1004</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47">
-        <v>4100</v>
+        <v>2000</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48">
-        <v>4100</v>
+        <v>2001</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49">
-        <v>4101</v>
+        <v>2002</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50">
-        <v>4102</v>
+        <v>2003</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D50" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51">
-        <v>4103</v>
+        <v>2004</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52">
-        <v>4104</v>
+        <v>3000</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
@@ -1471,63 +1579,203 @@
         <v>54</v>
       </c>
       <c r="D52" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53">
-        <v>5100</v>
+        <v>3001</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54">
-        <v>5101</v>
+        <v>3002</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55">
-        <v>5102</v>
+        <v>3003</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56">
+        <v>3004</v>
+      </c>
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>4100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>4100</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>4101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>4102</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>4103</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>4104</v>
+      </c>
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>5100</v>
+      </c>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>5101</v>
+      </c>
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>5102</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A66">
         <v>5103</v>
       </c>
-      <c r="B56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" t="s">
-        <v>52</v>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OP & ED Scene Add
</commit_message>
<xml_diff>
--- a/Assets/Resources/Data/Dialog.xlsx
+++ b/Assets/Resources/Data/Dialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Unity\capstone-2023-03\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B41968-A558-41C3-B00A-25E0F6AC1EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3047E9D5-9486-4388-9E2F-ED67D7CBB9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{E3E339C2-427C-46D8-B0F4-47F04CF9523A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Dialog!$A$1:$D$66</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Dialog!$A$1:$D$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -391,10 +391,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>내 라이브는… 이것으로 종료야.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>다음으로 내 제물이 될 사람이 너구나? 무대를 시작할 준비는 됐어?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -480,6 +476,54 @@
   </si>
   <si>
     <t>...죄송합니다 성녀님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 라이브는… 이것으로 종료.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 이긴… 건가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">으응. 축하해! 이번 ROAD TO V 대회의 우승자는 너야, 아이리. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전세계 사람들은 이제 모두 본인의 버츄얼 캐릭터를 이용해 교류하며\n\n현실에서 할 수 없는 일들을 쉽게 경험할 수 있는 가상현실의 인기는 날로 늘어가고\n\n가상의 인기는 곧 현실의 돈과 권력이 되는 시대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서기 2132년\n\n세계는 무구한 발전을 이룩하여, 완벽한 메타버스 세상에 돌입했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 최근 인기를 끄는 것은 바로\n\n본인의 캐릭터를 이용한 카드 배틀로얄 서바이벌 게임 'ROAD TO V'\n\n우승 조건은 단 하나, 가장 화려한 퍼포먼스를 선보이고 최후의 승자가 되어라!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 과연 올해의 우승자가 될 수 있을까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 여기 마녀 컨셉의 버츄얼 캐릭터인 당신, 아이리가 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이리는 훌륭하게 ROAD TO V 대회에서 우승.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수많은 부와 영예를 얻었고,\n\n그 이후에도 오랫동안 활동을 지속하며 가상 세계의 전설로 남게 되었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그녀를 동경하는 이들은 자신들을 '아이리스'라는 이름으로 부르며,\n\n 세대를 넘어 아이리의 이야기를 전했다고 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이해 주셔서 감사합니다 아ㅋㅋ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -512,20 +556,63 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -534,8 +621,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -569,10 +674,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}" name="Dialog" displayName="Dialog" ref="A1:D66" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D66" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
-    <sortCondition ref="A1:A66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}" name="Dialog" displayName="Dialog" ref="A1:D77" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D77" xr:uid="{0E257BDA-AC3B-4982-BEBE-D713DF32D959}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
+    <sortCondition ref="A1:A68"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1B7DBA41-96C3-4CE3-B474-58352C79090C}" uniqueName="1" name="index" queryTableFieldId="1"/>
@@ -881,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FB65A4-AFB1-47B1-836C-30EB70945D8C}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -921,7 +1026,7 @@
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -935,7 +1040,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -963,7 +1068,7 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -977,7 +1082,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -1131,7 +1236,7 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
@@ -1145,7 +1250,7 @@
         <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
@@ -1159,7 +1264,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
@@ -1417,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
@@ -1439,7 +1544,7 @@
         <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
@@ -1453,7 +1558,7 @@
         <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
@@ -1467,7 +1572,7 @@
         <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
@@ -1481,7 +1586,7 @@
         <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
@@ -1495,7 +1600,7 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
@@ -1509,7 +1614,7 @@
         <v>54</v>
       </c>
       <c r="D47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
@@ -1523,7 +1628,7 @@
         <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
@@ -1537,7 +1642,7 @@
         <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
@@ -1565,7 +1670,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
@@ -1579,7 +1684,7 @@
         <v>54</v>
       </c>
       <c r="D52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.4">
@@ -1593,7 +1698,7 @@
         <v>56</v>
       </c>
       <c r="D53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
@@ -1607,7 +1712,7 @@
         <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
@@ -1621,7 +1726,7 @@
         <v>58</v>
       </c>
       <c r="D55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.4">
@@ -1635,7 +1740,7 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.4">
@@ -1709,73 +1814,173 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>4104</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D62" t="s">
-        <v>83</v>
+      <c r="D62" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63">
-        <v>5100</v>
-      </c>
-      <c r="B63" t="s">
-        <v>39</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" t="s">
-        <v>62</v>
+        <v>4104</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64">
-        <v>5101</v>
+        <v>4104</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D64" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65">
-        <v>5102</v>
+        <v>5100</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66">
+        <v>5101</v>
+      </c>
+      <c r="B66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>5102</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A68">
         <v>5103</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B68" t="s">
         <v>42</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>14</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D68" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>6000</v>
+      </c>
+      <c r="D69" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>6000</v>
+      </c>
+      <c r="D70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>6000</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>6000</v>
+      </c>
+      <c r="D72" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>6000</v>
+      </c>
+      <c r="D73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>6001</v>
+      </c>
+      <c r="D74" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>6001</v>
+      </c>
+      <c r="D75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>6001</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>6001</v>
+      </c>
+      <c r="D77" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>